<commit_message>
Fixed adding shunt in Ymini
</commit_message>
<xml_diff>
--- a/ex_nr_ex1.xlsx
+++ b/ex_nr_ex1.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88275DAA-1798-9049-9C80-D5E702D0D5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B815337-5D54-FB43-ABE3-D9DFAB5E2DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="20920" windowHeight="14340" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="20920" windowHeight="14320" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
     <sheet name="line_imp" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,12 +48,6 @@
     <t>slack</t>
   </si>
   <si>
-    <t>pv</t>
-  </si>
-  <si>
-    <t>pq</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>shunt_r</t>
+  </si>
+  <si>
+    <t>shunt_x</t>
   </si>
 </sst>
 </file>
@@ -424,9 +424,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CC4DDF-8E3E-324E-AB44-8876A263AA5F}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -440,44 +440,35 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1.05</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1.04</v>
-      </c>
       <c r="E3">
-        <v>1</v>
+        <v>-0.6</v>
+      </c>
+      <c r="F3">
+        <v>-0.3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -485,13 +476,29 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>1.5</v>
+      <c r="E5">
+        <v>-0.6</v>
+      </c>
+      <c r="F5">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>-0.5</v>
+      </c>
+      <c r="F6">
+        <v>-0.4</v>
       </c>
     </row>
   </sheetData>
@@ -501,56 +508,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3C53D1-2A7C-F44F-B86A-DD1711AAE24B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>0.05</v>
       </c>
       <c r="C3">
+        <v>0.25</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>0.02</v>
+      </c>
+      <c r="C4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>23</v>
-      </c>
-      <c r="B4">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C4">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>3.3333000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>3.3333000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>0.01</v>
+      </c>
+      <c r="C6">
         <v>0.1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added transformer in excel
</commit_message>
<xml_diff>
--- a/ex_nr_ex1.xlsx
+++ b/ex_nr_ex1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A9DAD-7669-AE4B-8C01-9B270771B962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAE4AB5-46C9-B846-8495-443F673A10AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="20920" windowHeight="14320" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>bus_num</t>
   </si>
@@ -75,10 +75,10 @@
     <t>shunt_x</t>
   </si>
   <si>
-    <t>transformer</t>
-  </si>
-  <si>
-    <t>no</t>
+    <t>t_x</t>
+  </si>
+  <si>
+    <t>t_a</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,15 +514,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3C53D1-2A7C-F44F-B86A-DD1711AAE24B}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -541,8 +541,11 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12</v>
       </c>
@@ -558,11 +561,8 @@
       <c r="E2">
         <v>0.05</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>23</v>
       </c>
@@ -578,11 +578,8 @@
       <c r="E3">
         <v>0.05</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>14</v>
       </c>
@@ -598,11 +595,8 @@
       <c r="E4">
         <v>3.3333000000000002E-2</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
@@ -618,11 +612,8 @@
       <c r="E5">
         <v>3.3333000000000002E-2</v>
       </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>45</v>
       </c>
@@ -637,9 +628,6 @@
       </c>
       <c r="E6">
         <v>0.02</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed excel file and printing
</commit_message>
<xml_diff>
--- a/ex_nr_ex1.xlsx
+++ b/ex_nr_ex1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAE4AB5-46C9-B846-8495-443F673A10AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9036FCE-7159-E049-8E2D-5EC7AC9DC17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="20920" windowHeight="14320" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,7 +559,8 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.05</v>
+        <f>0.05/2</f>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -567,16 +568,19 @@
         <v>23</v>
       </c>
       <c r="B3">
-        <v>0.05</v>
+        <f>0.05/2</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C3">
-        <v>0.25</v>
+        <f>0.25/2</f>
+        <v>0.125</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.05</v>
+        <f>0.05/2/2</f>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -593,7 +597,8 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>3.3333000000000002E-2</v>
+        <f>0.033333/2</f>
+        <v>1.6666500000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -610,7 +615,8 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>3.3333000000000002E-2</v>
+        <f>0.033333/2</f>
+        <v>1.6666500000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -627,7 +633,8 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.02</v>
+        <f>0.02/2</f>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed around some iteration methods for NR and started on reactive power limits
</commit_message>
<xml_diff>
--- a/ex_nr_ex1.xlsx
+++ b/ex_nr_ex1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9036FCE-7159-E049-8E2D-5EC7AC9DC17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3CD8D6-C184-0041-B932-9131BB81C333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="20920" windowHeight="14320" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,8 +579,8 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <f>0.05/2/2</f>
-        <v>1.2500000000000001E-2</v>
+        <f>0.05/2</f>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
CHanged set initial guess method to take the values from t and v lists
</commit_message>
<xml_diff>
--- a/ex_nr_ex1.xlsx
+++ b/ex_nr_ex1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3CD8D6-C184-0041-B932-9131BB81C333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C0BA53-4C55-3F4E-9F54-4DEA3600C726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="20920" windowHeight="14320" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="20920" windowHeight="14320" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CC4DDF-8E3E-324E-AB44-8876A263AA5F}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,6 +462,12 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
@@ -470,6 +476,12 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
       <c r="E3">
         <v>-0.6</v>
       </c>
@@ -484,11 +496,23 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5">
         <v>-0.6</v>
       </c>
@@ -499,6 +523,12 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6">
         <v>-0.5</v>
@@ -516,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3C53D1-2A7C-F44F-B86A-DD1711AAE24B}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added reactive power limits. the correct function for this is NR_iterate_loop_qlim
</commit_message>
<xml_diff>
--- a/ex_nr_ex1.xlsx
+++ b/ex_nr_ex1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C0BA53-4C55-3F4E-9F54-4DEA3600C726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C323C66F-1CB3-EE4E-A322-612672E8E1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="20920" windowHeight="14320" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>bus_num</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>t_a</t>
+  </si>
+  <si>
+    <t>q_lim</t>
   </si>
 </sst>
 </file>
@@ -430,15 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CC4DDF-8E3E-324E-AB44-8876A263AA5F}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,8 +460,11 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -471,8 +477,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -489,7 +498,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -503,7 +512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -520,7 +529,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -547,7 +556,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,8 +618,8 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <f>0.05/2</f>
-        <v>2.5000000000000001E-2</v>
+        <f>0.05/2/2</f>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changed around pflow and qflow. still not quite working, need to fix formula.
</commit_message>
<xml_diff>
--- a/ex_nr_ex1.xlsx
+++ b/ex_nr_ex1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851DC2DC-490C-AB46-A2FF-01E6AC3566C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9025B00A-8618-E047-83F4-5531B281AA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="20920" windowHeight="14320" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,10 +553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3C53D1-2A7C-F44F-B86A-DD1711AAE24B}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,42 +607,40 @@
         <v>23</v>
       </c>
       <c r="B3">
+        <v>0.05</v>
+      </c>
+      <c r="C3">
+        <v>0.25</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <f>0.05/2</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C3">
-        <f>0.25/2</f>
-        <v>0.125</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f>0.05/2/2</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B4">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="C4">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <f>0.033333/2</f>
-        <v>1.6666500000000001E-2</v>
+        <f>0.05/2</f>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>0.02</v>
@@ -660,18 +658,36 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>0.02</v>
+      </c>
+      <c r="C6">
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>0.033333/2</f>
+        <v>1.6666500000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>45</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>0.01</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>0.1</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <f>0.02/2</f>
         <v>0.01</v>
       </c>

</xml_diff>